<commit_message>
guarda registross en base de datos, crea otra tabla para guardar los terceros
</commit_message>
<xml_diff>
--- a/registros_excel/2024-02-07.xlsx
+++ b/registros_excel/2024-02-07.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,216 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1053868254</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tatiana Pachon</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>13:28:28</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>13:28:28</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>13:28:28</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1015463003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Leonardo Maje</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>13:36:18</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>13:36:18</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13:36:18</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1054398414</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Julian Largo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>13:41:18</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>13:41:18</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>13:41:18</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10101010</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Proveedor</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Tercero</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14:13:10</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>14:13:10</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>14:13:10</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1054398414</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Julian Largo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14:15:28</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>13:41:18</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>14:15:28</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
genera codigo qr y guarda el registro en la base de datos
</commit_message>
<xml_diff>
--- a/registros_excel/2024-02-07.xlsx
+++ b/registros_excel/2024-02-07.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -902,6 +902,48 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10541212</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>prueba Proveedor 2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Tercero</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16:57:55</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16:38:14</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>16:57:55</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Salida PM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>